<commit_message>
Dataset WIP.  contact and customer SQL datafiles with and without backticks.  CSV files for ingredients, paytmentType state Sales tax and extra ingredients.
</commit_message>
<xml_diff>
--- a/datasets/98-Pizza Datasets v170517.xlsx
+++ b/datasets/98-Pizza Datasets v170517.xlsx
@@ -5,12 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glenn-daviddaniel/Documents/lgProjects/gc98/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glenn-daviddaniel/Documents/lgProjects/gc98/98-Pizza/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="-21140" windowWidth="17140" windowHeight="21140" tabRatio="500"/>
-    <workbookView xWindow="-6900" yWindow="-21600" windowWidth="38400" windowHeight="21600" tabRatio="500" firstSheet="15" activeTab="16"/>
+    <workbookView minimized="1" xWindow="-6900" yWindow="-21140" windowWidth="14780" windowHeight="21140" tabRatio="500" firstSheet="15" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Tables (2)" sheetId="2" r:id="rId1"/>
@@ -18,9 +17,9 @@
     <sheet name="user" sheetId="3" r:id="rId3"/>
     <sheet name="checkingAcct" sheetId="4" r:id="rId4"/>
     <sheet name="creditCardAcct" sheetId="20" r:id="rId5"/>
-    <sheet name="contact" sheetId="8" r:id="rId6"/>
-    <sheet name="customerProfile" sheetId="15" r:id="rId7"/>
-    <sheet name="customer" sheetId="5" r:id="rId8"/>
+    <sheet name="customer" sheetId="5" r:id="rId6"/>
+    <sheet name="contact" sheetId="8" r:id="rId7"/>
+    <sheet name="customerProfile" sheetId="15" r:id="rId8"/>
     <sheet name="otherProduct" sheetId="17" r:id="rId9"/>
     <sheet name="recipe" sheetId="18" r:id="rId10"/>
     <sheet name="deliveryAddress" sheetId="6" r:id="rId11"/>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2454" uniqueCount="514">
   <si>
     <t>-- Tue May 16 14:24:41 2017</t>
   </si>
@@ -1588,6 +1587,9 @@
   </si>
   <si>
     <t>maxLocalTaxRate</t>
+  </si>
+  <si>
+    <t>createDateTime</t>
   </si>
 </sst>
 </file>
@@ -1597,7 +1599,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1646,13 +1648,26 @@
       <color rgb="FF006621"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1686,7 +1701,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1702,6 +1717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1998,12 +2014,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F213"/>
+  <dimension ref="A1:F216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B171" activeCellId="1" sqref="B195:B199 B171"/>
-    </sheetView>
-    <sheetView topLeftCell="A2" workbookViewId="1">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A149" sqref="A149"/>
       <selection pane="topRight" activeCell="A20" sqref="A20"/>
@@ -2012,7 +2025,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2036,7 +2050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="str">
         <f>C2</f>
         <v>idCustomer</v>
@@ -2048,9 +2062,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B10" si="0">C3</f>
+        <f t="shared" ref="B3:B13" si="0">C3</f>
         <v>customerName</v>
       </c>
       <c r="C3" t="s">
@@ -2060,661 +2074,643 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B4" t="str">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>user_idUserName</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C7" t="s">
         <v>79</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B5" t="str">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>creditCard1ID</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
         <v>80</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B6" t="str">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>creditCard2ID</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B7" t="str">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>creditCard3ID</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" t="s">
         <v>83</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B8" t="str">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>checkingAcctID</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>84</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D11" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B9" t="str">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>checkingAcct_idcheckingAcct</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C12" t="s">
         <v>85</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B10" t="str">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>contact_idcontacts</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>86</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>470</v>
       </c>
-      <c r="B12" s="6" t="str">
-        <f>C12&amp;D12&amp;E12</f>
+      <c r="B15" s="6" t="str">
+        <f>C15&amp;D15&amp;E15</f>
         <v>PizzaPicadilly.user</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E15" t="s">
         <v>20</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B13" t="str">
-        <f>C13</f>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="str">
+        <f>C16</f>
         <v>idUserName</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B14" t="str">
-        <f t="shared" ref="B14:B18" si="1">C14</f>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="str">
+        <f t="shared" ref="B17:B21" si="1">C17</f>
         <v>idCustomer</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>26</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B15" t="str">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="str">
         <f t="shared" si="1"/>
         <v>username</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>28</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B16" t="str">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="str">
         <f t="shared" si="1"/>
         <v>email</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B17" t="str">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="str">
         <f t="shared" si="1"/>
         <v>password</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B18" t="str">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="str">
         <f t="shared" si="1"/>
         <v>create_time</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>34</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>470</v>
       </c>
-      <c r="B20" s="6" t="str">
-        <f>C20&amp;D20&amp;E20</f>
+      <c r="B23" s="6" t="str">
+        <f>C23&amp;D23&amp;E23</f>
         <v>PizzaPicadilly.contact</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>15</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D23" t="s">
         <v>19</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E23" t="s">
         <v>54</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B21" t="str">
-        <f>C21</f>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="str">
+        <f>C24</f>
         <v>idContact</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>55</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D24" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B22" t="str">
-        <f t="shared" ref="B22:B32" si="2">C22</f>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="str">
+        <f t="shared" ref="B25:B35" si="2">C25</f>
         <v>contactType</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>57</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B23" t="str">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="str">
         <f t="shared" si="2"/>
         <v>contactStreet1</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C26" t="s">
         <v>59</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B24" t="str">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="str">
         <f t="shared" si="2"/>
         <v>contactStreet2</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C27" t="s">
         <v>60</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B25" t="str">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="str">
         <f t="shared" si="2"/>
         <v>contactCity</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" t="s">
         <v>61</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B26" t="str">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="str">
         <f t="shared" si="2"/>
         <v>contactState</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>62</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B27" t="str">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="str">
         <f t="shared" si="2"/>
         <v>contactZip</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>64</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D30" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B28" t="str">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="str">
         <f t="shared" si="2"/>
         <v>contactPhone1</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C31" t="s">
         <v>66</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B29" t="str">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="str">
         <f t="shared" si="2"/>
         <v>contactPhone2</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C32" t="s">
         <v>67</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B30" t="str">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="str">
         <f t="shared" si="2"/>
         <v>contactEmail</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" t="s">
         <v>68</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B31" t="str">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="str">
         <f t="shared" si="2"/>
         <v>idCustomer</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C34" t="s">
         <v>26</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B32" t="str">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B35" t="str">
         <f t="shared" si="2"/>
         <v>idSupplier</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C35" t="s">
         <v>116</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D35" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>470</v>
       </c>
-      <c r="B34" s="6" t="str">
-        <f>C34&amp;D34&amp;E34</f>
+      <c r="B37" s="6" t="str">
+        <f>C37&amp;D37&amp;E37</f>
         <v>PizzaPicadilly.creditCard</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C37" t="s">
         <v>15</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D37" t="s">
         <v>19</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E37" t="s">
         <v>244</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F37" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B35" t="str">
-        <f>C35</f>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="str">
+        <f>C38</f>
         <v>idcreditCards</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C38" t="s">
         <v>245</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D38" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B36" t="str">
-        <f t="shared" ref="B36:B45" si="3">C36</f>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B39" t="str">
+        <f t="shared" ref="B39:B48" si="3">C39</f>
         <v>cardNumber</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C39" t="s">
         <v>246</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B37" t="str">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="str">
         <f t="shared" si="3"/>
         <v>cvvNumber</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C40" t="s">
         <v>247</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D40" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B38" t="str">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="str">
         <f t="shared" si="3"/>
         <v>cardName</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>248</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D41" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B39" t="str">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B42" t="str">
         <f t="shared" si="3"/>
         <v>billStreet</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" t="s">
         <v>249</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B40" t="str">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B43" t="str">
         <f t="shared" si="3"/>
         <v>billCity</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C43" t="s">
         <v>250</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B41" t="str">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="str">
         <f t="shared" si="3"/>
         <v>billState</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C44" t="s">
         <v>251</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B42" t="str">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="str">
         <f t="shared" si="3"/>
         <v>billZip</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C45" t="s">
         <v>252</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D45" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B43" t="str">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="str">
         <f t="shared" si="3"/>
         <v>idCustomer</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C46" t="s">
         <v>26</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D46" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B44" t="str">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="str">
         <f t="shared" si="3"/>
         <v>customer_idCustomer</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C47" t="s">
         <v>146</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D47" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B45" t="str">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B48" t="str">
         <f t="shared" si="3"/>
         <v>customer_user_idUserName</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C48" t="s">
         <v>147</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D48" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>470</v>
       </c>
-      <c r="B47" s="6" t="str">
-        <f>C47&amp;D47&amp;E47</f>
+      <c r="B50" s="6" t="str">
+        <f>C50&amp;D50&amp;E50</f>
         <v>PizzaPicadilly.checkingAcct</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C50" t="s">
         <v>15</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D50" t="s">
         <v>19</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E50" t="s">
         <v>38</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F50" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B48" t="str">
-        <f>C48</f>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="str">
+        <f>C51</f>
         <v>idcheckingAcct</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C51" t="s">
         <v>39</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D51" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B49" t="str">
-        <f t="shared" ref="B49:B56" si="4">C49</f>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="str">
+        <f t="shared" ref="B52:B59" si="4">C52</f>
         <v>bankNumber</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C52" t="s">
         <v>40</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D52" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B50" t="str">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="str">
         <f t="shared" si="4"/>
         <v>acctNumber</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C53" t="s">
         <v>42</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B51" t="str">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="str">
         <f t="shared" si="4"/>
         <v>acctHolderName</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C54" t="s">
         <v>43</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D54" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B52" t="str">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="str">
         <f t="shared" si="4"/>
         <v>acctStreet</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C55" t="s">
         <v>45</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D55" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B53" t="str">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B56" t="str">
         <f t="shared" si="4"/>
         <v>acctCity</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C56" t="s">
         <v>46</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D56" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B54" t="str">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57" t="str">
         <f t="shared" si="4"/>
         <v>acctState</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C57" t="s">
         <v>47</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B55" t="str">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B58" t="str">
         <f t="shared" si="4"/>
         <v>acctZip</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C58" t="s">
         <v>48</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D58" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B56" t="str">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B59" t="str">
         <f t="shared" si="4"/>
         <v>idCustomer</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C59" t="s">
         <v>26</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D59" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>470</v>
-      </c>
-      <c r="B58" s="6" t="str">
-        <f>C58&amp;D58&amp;E58</f>
-        <v>PizzaPicadilly.CustomerProfile</v>
-      </c>
-      <c r="C58" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" t="s">
-        <v>19</v>
-      </c>
-      <c r="E58" t="s">
-        <v>73</v>
-      </c>
-      <c r="F58" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B59" t="str">
-        <f>C59</f>
-        <v>idCustomerProfile</v>
-      </c>
-      <c r="C59" t="s">
-        <v>74</v>
-      </c>
-      <c r="D59" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2723,7 +2719,7 @@
       </c>
       <c r="B61" s="6" t="str">
         <f>C61&amp;D61&amp;E61</f>
-        <v>PizzaPicadilly.deliveryAddress</v>
+        <v>PizzaPicadilly.CustomerProfile</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
@@ -2732,1399 +2728,1396 @@
         <v>19</v>
       </c>
       <c r="E61" t="s">
-        <v>136</v>
+        <v>73</v>
       </c>
       <c r="F61" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B62" t="str">
         <f>C62</f>
+        <v>idCustomerProfile</v>
+      </c>
+      <c r="C62" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>470</v>
+      </c>
+      <c r="B64" s="6" t="str">
+        <f>C64&amp;D64&amp;E64</f>
+        <v>PizzaPicadilly.deliveryAddress</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" t="s">
+        <v>136</v>
+      </c>
+      <c r="F64" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B65" t="str">
+        <f>C65</f>
         <v>idDelivery</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C65" t="s">
         <v>137</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D65" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B63" t="str">
-        <f t="shared" ref="B63:B74" si="5">C63</f>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B66" t="str">
+        <f t="shared" ref="B66:B77" si="5">C66</f>
         <v>deliveryStreet1</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C66" t="s">
         <v>138</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D66" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B64" t="str">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B67" t="str">
         <f t="shared" si="5"/>
         <v>deliveryStreet2</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C67" t="s">
         <v>139</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D67" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B65" t="str">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B68" t="str">
         <f t="shared" si="5"/>
         <v>deliveryCity</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C68" t="s">
         <v>140</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D68" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B66" t="str">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B69" t="str">
         <f t="shared" si="5"/>
         <v>deliveryState</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C69" t="s">
         <v>141</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D69" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B67" t="str">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B70" t="str">
         <f t="shared" si="5"/>
         <v>deliveryZip</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C70" t="s">
         <v>142</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D70" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B68" t="str">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B71" t="str">
         <f t="shared" si="5"/>
         <v>deliveryPhone1</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C71" t="s">
         <v>143</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D71" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B69" t="str">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B72" t="str">
         <f t="shared" si="5"/>
         <v>deliveryPhone2</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C72" t="s">
         <v>144</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D72" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B70" t="str">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B73" t="str">
         <f t="shared" si="5"/>
         <v>idCustomer</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C73" t="s">
         <v>26</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D73" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B71" t="str">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B74" t="str">
         <f t="shared" si="5"/>
         <v>customer_idCustomer</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C74" t="s">
         <v>146</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D74" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B72" t="str">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B75" t="str">
         <f t="shared" si="5"/>
         <v>customer_user_idUserName</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C75" t="s">
         <v>147</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D75" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B73" t="str">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B76" t="str">
         <f t="shared" si="5"/>
         <v>customer_checkingAcct_idcheckingAcct</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C76" t="s">
         <v>148</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B74" t="str">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B77" t="str">
         <f t="shared" si="5"/>
         <v>customer_contact_idcontacts</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C77" t="s">
         <v>149</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D77" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>470</v>
       </c>
-      <c r="B76" s="6" t="str">
-        <f>C76&amp;D76&amp;E76</f>
+      <c r="B79" s="6" t="str">
+        <f>C79&amp;D79&amp;E79</f>
         <v>PizzaPicadilly.paymentType</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C79" t="s">
         <v>15</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D79" t="s">
         <v>19</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E79" t="s">
         <v>154</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F79" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B77" t="str">
-        <f>C77</f>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B80" t="str">
+        <f>C80</f>
         <v>idpaymentType</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C80" t="s">
         <v>155</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D80" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B78" t="str">
-        <f t="shared" ref="B78:B79" si="6">C78</f>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B81" t="str">
+        <f t="shared" ref="B81:B82" si="6">C81</f>
         <v>paymentType</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C81" t="s">
         <v>154</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D81" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B79" t="str">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B82" t="str">
         <f t="shared" si="6"/>
         <v>idCustomer</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C82" t="s">
         <v>26</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D82" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>470</v>
       </c>
-      <c r="B81" s="6" t="str">
-        <f>C81&amp;D81&amp;E81</f>
+      <c r="B84" s="6" t="str">
+        <f>C84&amp;D84&amp;E84</f>
         <v>PizzaPicadilly.otherProduct</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C84" t="s">
         <v>15</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D84" t="s">
         <v>19</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E84" t="s">
         <v>108</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F84" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B82" t="str">
-        <f>C82</f>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B85" t="str">
+        <f>C85</f>
         <v>idotherProducts</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C85" t="s">
         <v>109</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D85" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B83" t="str">
-        <f t="shared" ref="B83:B92" si="7">C83</f>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B86" t="str">
+        <f t="shared" ref="B86:B95" si="7">C86</f>
         <v>productType</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C86" t="s">
         <v>111</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D86" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B84" t="str">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B87" t="str">
         <f t="shared" si="7"/>
         <v>productName</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C87" t="s">
         <v>113</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D87" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B85" t="str">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B88" t="str">
         <f t="shared" si="7"/>
         <v>Description</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C88" t="s">
         <v>114</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D88" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B86" t="str">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B89" t="str">
         <f t="shared" si="7"/>
         <v>Brand</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C89" t="s">
         <v>115</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D89" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B87" t="str">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B90" t="str">
         <f t="shared" si="7"/>
         <v>idSupplier</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C90" t="s">
         <v>116</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D90" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B88" t="str">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B91" t="str">
         <f t="shared" si="7"/>
         <v>Cost</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C91" t="s">
         <v>117</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D91" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B89" t="str">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B92" t="str">
         <f t="shared" si="7"/>
         <v>Price</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C92" t="s">
         <v>119</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D92" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B90" t="str">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B93" t="str">
         <f t="shared" si="7"/>
         <v>Markup</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C93" t="s">
         <v>120</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D93" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B91" t="str">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B94" t="str">
         <f t="shared" si="7"/>
         <v>barCode</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C94" t="s">
         <v>122</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D94" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B92" t="str">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B95" t="str">
         <f t="shared" si="7"/>
         <v>productSKU</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C95" t="s">
         <v>124</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D95" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B94" s="6" t="str">
-        <f>C94&amp;D94&amp;E94</f>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B97" s="6" t="str">
+        <f>C97&amp;D97&amp;E97</f>
         <v>PizzaPicadilly.pizzaProduct</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C97" t="s">
         <v>15</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D97" t="s">
         <v>19</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E97" t="s">
         <v>235</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F97" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B95" t="str">
-        <f>C95</f>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B98" t="str">
+        <f>C98</f>
         <v>idpizzaProducts</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C98" t="s">
         <v>236</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D98" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B96" t="str">
-        <f t="shared" ref="B96:B99" si="8">C96</f>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B99" t="str">
+        <f t="shared" ref="B99:B102" si="8">C99</f>
         <v>pizzaName</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C99" t="s">
         <v>130</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D99" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B97" t="str">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B100" t="str">
         <f t="shared" si="8"/>
         <v>idRecipe</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C100" t="s">
         <v>186</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D100" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B98" t="str">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B101" t="str">
         <f t="shared" si="8"/>
         <v>recipe_idRecipes</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C101" t="s">
         <v>237</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D101" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B99" t="str">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B102" t="str">
         <f t="shared" si="8"/>
         <v>pieType_idpieType</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C102" t="s">
         <v>238</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D102" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>470</v>
       </c>
-      <c r="B101" s="6" t="str">
-        <f>C101&amp;D101&amp;E101</f>
+      <c r="B104" s="6" t="str">
+        <f>C104&amp;D104&amp;E104</f>
         <v>PizzaPicadilly.pieType</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C104" t="s">
         <v>15</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D104" t="s">
         <v>19</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E104" t="s">
         <v>216</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F104" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B102" t="str">
-        <f>C102</f>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B105" t="str">
+        <f>C105</f>
         <v>idpieType</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C105" t="s">
         <v>217</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D105" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B103" t="str">
-        <f t="shared" ref="B103:B116" si="9">C103</f>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B106" t="str">
+        <f t="shared" ref="B106:B119" si="9">C106</f>
         <v>pieTypeName</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C106" t="s">
         <v>290</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D106" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B104" t="str">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B107" t="str">
         <f t="shared" si="9"/>
         <v>order_idorder</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C107" t="s">
         <v>220</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D107" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B105" t="str">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B108" t="str">
         <f t="shared" si="9"/>
         <v>order_customer_idCustomer</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C108" t="s">
         <v>221</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D108" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B106" t="str">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B109" t="str">
         <f t="shared" si="9"/>
         <v>order_customer_user_idUserName</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C109" t="s">
         <v>222</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D109" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B107" t="str">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B110" t="str">
         <f t="shared" si="9"/>
         <v>order_customer_checkingAcct_idcheckingAcct</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C110" t="s">
         <v>223</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D110" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B108" t="str">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B111" t="str">
         <f t="shared" si="9"/>
         <v>order_customer_contact_idcontacts</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C111" t="s">
         <v>224</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D111" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B109" t="str">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B112" t="str">
         <f t="shared" si="9"/>
         <v>order_deliveryAddress_idDelivery</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C112" t="s">
         <v>225</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D112" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B110" t="str">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B113" t="str">
         <f t="shared" si="9"/>
         <v>order_deliveryAddress_customer_idCustomer</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C113" t="s">
         <v>226</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D113" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B111" t="str">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B114" t="str">
         <f t="shared" si="9"/>
         <v>order_deliveryAddress_customer_user_idUserName</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C114" t="s">
         <v>227</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D114" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B112" t="str">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B115" t="str">
         <f t="shared" si="9"/>
         <v>order_deliveryAddress_customer_checkingAcct_idcheckingAcct</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C115" t="s">
         <v>228</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D115" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B113" t="str">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B116" t="str">
         <f t="shared" si="9"/>
         <v>order_deliveryAddress_customer_contact_idcontacts</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C116" t="s">
         <v>229</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D116" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B114" t="str">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B117" t="str">
         <f t="shared" si="9"/>
         <v>order_contact_idContact</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C117" t="s">
         <v>230</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D117" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B115" t="str">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B118" t="str">
         <f t="shared" si="9"/>
         <v>order_paymentType_idpaymentType</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C118" t="s">
         <v>231</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D118" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B116" t="str">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B119" t="str">
         <f t="shared" si="9"/>
         <v>order_otherProduct_idotherProducts</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C119" t="s">
         <v>232</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D119" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>470</v>
       </c>
-      <c r="B118" s="6" t="str">
-        <f>C118&amp;D118&amp;E118</f>
+      <c r="B121" s="6" t="str">
+        <f>C121&amp;D121&amp;E121</f>
         <v>PizzaPicadilly.recipe</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C121" t="s">
         <v>15</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D121" t="s">
         <v>19</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E121" t="s">
         <v>127</v>
       </c>
-      <c r="F118" t="s">
+      <c r="F121" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B119" t="str">
-        <f>C119</f>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B122" t="str">
+        <f>C122</f>
         <v>idRecipes</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C122" t="s">
         <v>128</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D122" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B120" t="str">
-        <f t="shared" ref="B120:B123" si="10">C120</f>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B123" t="str">
+        <f t="shared" ref="B123:B126" si="10">C123</f>
         <v>pizzaName</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C123" t="s">
         <v>130</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D123" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B121" t="str">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B124" t="str">
         <f t="shared" si="10"/>
         <v>crustStandard</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C124" t="s">
         <v>132</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D124" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B122" t="str">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B125" t="str">
         <f t="shared" si="10"/>
         <v>cheeseType</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C125" t="s">
         <v>133</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D125" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B123" t="str">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B126" t="str">
         <f t="shared" si="10"/>
         <v>toppings</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C126" t="s">
         <v>134</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D126" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>470</v>
       </c>
-      <c r="B125" s="6" t="str">
-        <f>C125&amp;D125&amp;E125</f>
+      <c r="B128" s="6" t="str">
+        <f>C128&amp;D128&amp;E128</f>
         <v>PizzaPicadilly.Ingredient</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C128" t="s">
         <v>15</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D128" t="s">
         <v>19</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E128" t="s">
         <v>451</v>
       </c>
-      <c r="F125" t="s">
+      <c r="F128" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B126" t="str">
-        <f>C126</f>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B129" t="str">
+        <f>C129</f>
         <v>idIngredient</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C129" t="s">
         <v>452</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D129" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B127" t="str">
-        <f t="shared" ref="B127:B134" si="11">C127</f>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B130" t="str">
+        <f t="shared" ref="B130:B137" si="11">C130</f>
         <v>ingredientName</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C130" t="s">
         <v>171</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D130" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B128" t="str">
-        <f>C128</f>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B131" t="str">
+        <f>C131</f>
         <v>productSKU</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C131" t="s">
         <v>124</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D131" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B129" t="str">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B132" t="str">
         <f t="shared" si="11"/>
         <v>costPerOz</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C132" t="s">
         <v>172</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D132" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B130" t="str">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B133" t="str">
         <f t="shared" si="11"/>
         <v>ozInSmall</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C133" t="s">
         <v>173</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D133" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B131" t="str">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B134" t="str">
         <f t="shared" si="11"/>
         <v>ozInMedium</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C134" t="s">
         <v>174</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D134" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B132" t="str">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B135" t="str">
         <f t="shared" si="11"/>
         <v>ozInLarge</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C135" t="s">
         <v>175</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D135" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B133" t="str">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B136" t="str">
         <f t="shared" si="11"/>
         <v>ozInExtraLarge</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C136" t="s">
         <v>176</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D136" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B134" t="str">
+    <row r="137" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B137" t="str">
         <f t="shared" si="11"/>
         <v>idSupplier</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C137" t="s">
         <v>116</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D137" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>470</v>
       </c>
-      <c r="B136" s="6" t="str">
-        <f>C136&amp;D136&amp;E136</f>
+      <c r="B139" s="6" t="str">
+        <f>C139&amp;D139&amp;E139</f>
         <v>PizzaPicadilly.orderExtraIngredientList</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C139" t="s">
         <v>15</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D139" t="s">
         <v>19</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E139" t="s">
         <v>471</v>
       </c>
-      <c r="F136" t="s">
+      <c r="F139" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B137" t="str">
-        <f>C137</f>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B140" t="str">
+        <f>C140</f>
         <v>idExtraIngredient</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C140" t="s">
         <v>297</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D140" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B138" t="str">
-        <f t="shared" ref="B138:B139" si="12">C138</f>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B141" t="str">
+        <f t="shared" ref="B141:B142" si="12">C141</f>
         <v>ingredients</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C141" t="s">
         <v>180</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D141" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B139" t="str">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B142" t="str">
         <f t="shared" si="12"/>
         <v>Ingredients_idIngredients</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C142" t="s">
         <v>181</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D142" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B141" s="6" t="str">
-        <f>C141&amp;D141&amp;E141</f>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B144" s="6" t="str">
+        <f>C144&amp;D144&amp;E144</f>
         <v>PizzaPicadilly.productSupplier</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C144" t="s">
         <v>15</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D144" t="s">
         <v>19</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E144" t="s">
         <v>256</v>
       </c>
-      <c r="F141" t="s">
+      <c r="F144" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B142" t="str">
-        <f>C142</f>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B145" t="str">
+        <f>C145</f>
         <v>idSupplier</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C145" t="s">
         <v>116</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D145" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B143" t="str">
-        <f t="shared" ref="B143:B145" si="13">C143</f>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B146" t="str">
+        <f t="shared" ref="B146:B148" si="13">C146</f>
         <v>supplierName</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C146" t="s">
         <v>257</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D146" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B144" t="str">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B147" t="str">
         <f t="shared" si="13"/>
         <v>idContact</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C147" t="s">
         <v>55</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D147" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B145" t="str">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B148" t="str">
         <f t="shared" si="13"/>
         <v>productSKU</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C148" t="s">
         <v>124</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D148" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>470</v>
       </c>
-      <c r="B147" s="6" t="str">
-        <f>C147&amp;D147&amp;E147</f>
+      <c r="B150" s="6" t="str">
+        <f>C150&amp;D150&amp;E150</f>
         <v>PizzaPicadilly.order</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C150" t="s">
         <v>15</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D150" t="s">
         <v>19</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E150" t="s">
         <v>184</v>
       </c>
-      <c r="F147" t="s">
+      <c r="F150" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B148" t="str">
-        <f>C148</f>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B151" t="str">
+        <f>C151</f>
         <v>idorder</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C151" t="s">
         <v>185</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D151" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B149" t="str">
-        <f t="shared" ref="B149:B170" si="14">C149</f>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B152" t="str">
+        <f t="shared" ref="B152:B173" si="14">C152</f>
         <v>pizzaCode</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C152" t="s">
         <v>162</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D152" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B150" t="str">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B153" t="str">
         <f t="shared" si="14"/>
         <v>productName</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C153" t="s">
         <v>113</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D153" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B151" t="str">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B154" t="str">
         <f t="shared" si="14"/>
         <v>idRecipe</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C154" t="s">
         <v>186</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D154" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B152" t="str">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B155" t="str">
         <f t="shared" si="14"/>
         <v>size</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C155" t="s">
         <v>187</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D155" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B153" t="str">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B156" t="str">
         <f t="shared" si="14"/>
         <v>crustType</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C156" t="s">
         <v>188</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D156" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B154" t="str">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B157" t="str">
         <f t="shared" si="14"/>
         <v>customer_idCustomer</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C157" t="s">
         <v>146</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D157" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B155" t="str">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B158" t="str">
         <f t="shared" si="14"/>
         <v>customer_user_idUserName</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C158" t="s">
         <v>147</v>
       </c>
-      <c r="D155" t="s">
+      <c r="D158" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B156" t="str">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B159" t="str">
         <f t="shared" si="14"/>
         <v>customer_checkingAcct_idcheckingAcct</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C159" t="s">
         <v>148</v>
       </c>
-      <c r="D156" t="s">
+      <c r="D159" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B157" t="str">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B160" t="str">
         <f t="shared" si="14"/>
         <v>customer_contact_idcontacts</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C160" t="s">
         <v>149</v>
       </c>
-      <c r="D157" t="s">
+      <c r="D160" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B158" t="str">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B161" t="str">
         <f t="shared" si="14"/>
         <v>idDeliveryAddress</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C161" t="s">
         <v>189</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D161" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B159" t="str">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B162" t="str">
         <f t="shared" si="14"/>
         <v>idOtherProducts</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C162" t="s">
         <v>190</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D162" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B160" t="str">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B163" t="str">
         <f t="shared" si="14"/>
         <v>quantity</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C163" t="s">
         <v>191</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D163" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B161" t="str">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B164" t="str">
         <f t="shared" si="14"/>
         <v>deliveryAddress_idDelivery</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C164" t="s">
         <v>192</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D164" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B162" t="str">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B165" t="str">
         <f t="shared" si="14"/>
         <v>deliveryAddress_customer_idCustomer</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C165" t="s">
         <v>193</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D165" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B163" t="str">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B166" t="str">
         <f t="shared" si="14"/>
         <v>deliveryAddress_customer_user_idUserName</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C166" t="s">
         <v>194</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D166" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B164" t="str">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B167" t="str">
         <f t="shared" si="14"/>
         <v>deliveryAddress_customer_checkingAcct_idcheckingAcct</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C167" t="s">
         <v>195</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D167" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B165" t="str">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B168" t="str">
         <f t="shared" si="14"/>
         <v>deliveryAddress_customer_contact_idcontacts</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C168" t="s">
         <v>196</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D168" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B166" t="str">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B169" t="str">
         <f t="shared" si="14"/>
         <v>contact_idContact</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C169" t="s">
         <v>197</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D169" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B167" t="str">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B170" t="str">
         <f t="shared" si="14"/>
         <v>paymentType_idpaymentType</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C170" t="s">
         <v>198</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D170" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B168" t="str">
-        <f>C168</f>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B171" t="str">
+        <f>C171</f>
         <v>otherProduct_idotherProducts</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C171" t="s">
         <v>199</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D171" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B169" t="str">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B172" t="str">
         <f t="shared" si="14"/>
         <v>pizzaPriceList_idpizzaPriceList</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C172" t="s">
         <v>200</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D172" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B170" t="str">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B173" t="str">
         <f t="shared" si="14"/>
         <v>extraIngredientList_idaddOn</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C173" t="s">
         <v>201</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D173" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A172" t="s">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
         <v>470</v>
       </c>
-      <c r="B172" s="6" t="str">
-        <f>C172&amp;D172&amp;E172</f>
+      <c r="B175" s="6" t="str">
+        <f>C175&amp;D175&amp;E175</f>
         <v>PizzaPicadilly.PriceList</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C175" t="s">
         <v>15</v>
       </c>
-      <c r="D172" t="s">
+      <c r="D175" t="s">
         <v>19</v>
       </c>
-      <c r="E172" t="s">
+      <c r="E175" t="s">
         <v>472</v>
       </c>
-      <c r="F172" t="s">
+      <c r="F175" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B173" t="str">
-        <f>C173</f>
-        <v>idPriceList</v>
-      </c>
-      <c r="C173" t="s">
-        <v>473</v>
-      </c>
-      <c r="D173" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B174" t="str">
-        <f t="shared" ref="B174:B180" si="15">C174</f>
-        <v>idPizzaProduct</v>
-      </c>
-      <c r="C174" t="s">
-        <v>160</v>
-      </c>
-      <c r="D174" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B175" t="str">
-        <f t="shared" si="15"/>
-        <v>pieSize</v>
-      </c>
-      <c r="C175" t="s">
-        <v>161</v>
-      </c>
-      <c r="D175" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B176" t="str">
-        <f t="shared" si="15"/>
-        <v>pizzaCode</v>
+        <f>C176</f>
+        <v>idPriceList</v>
       </c>
       <c r="C176" t="s">
-        <v>162</v>
+        <v>473</v>
       </c>
       <c r="D176" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B177" t="str">
-        <f t="shared" si="15"/>
-        <v>pizzaCost</v>
+        <f t="shared" ref="B177:B183" si="15">C177</f>
+        <v>idPizzaProduct</v>
       </c>
       <c r="C177" t="s">
-        <v>474</v>
+        <v>160</v>
       </c>
       <c r="D177" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B178" t="str">
         <f t="shared" si="15"/>
-        <v>pizzaMarkup</v>
+        <v>pieSize</v>
       </c>
       <c r="C178" t="s">
-        <v>475</v>
+        <v>161</v>
       </c>
       <c r="D178" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B179" t="str">
         <f t="shared" si="15"/>
-        <v>pizzaDiscount</v>
+        <v>pizzaCode</v>
       </c>
       <c r="C179" t="s">
-        <v>476</v>
+        <v>162</v>
       </c>
       <c r="D179" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B180" t="str">
         <f t="shared" si="15"/>
-        <v>pizzaPrice</v>
+        <v>pizzaCost</v>
       </c>
       <c r="C180" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D180" t="s">
         <v>118</v>
@@ -4132,11 +4125,11 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B181" t="str">
-        <f t="shared" ref="B181:B184" si="16">C181</f>
-        <v>otherCost</v>
+        <f t="shared" si="15"/>
+        <v>pizzaMarkup</v>
       </c>
       <c r="C181" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="D181" t="s">
         <v>118</v>
@@ -4144,370 +4137,406 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B182" t="str">
+        <f t="shared" si="15"/>
+        <v>pizzaDiscount</v>
+      </c>
+      <c r="C182" t="s">
+        <v>476</v>
+      </c>
+      <c r="D182" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B183" t="str">
+        <f t="shared" si="15"/>
+        <v>pizzaPrice</v>
+      </c>
+      <c r="C183" t="s">
+        <v>477</v>
+      </c>
+      <c r="D183" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B184" t="str">
+        <f t="shared" ref="B184:B187" si="16">C184</f>
+        <v>otherCost</v>
+      </c>
+      <c r="C184" t="s">
+        <v>481</v>
+      </c>
+      <c r="D184" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B185" t="str">
         <f t="shared" si="16"/>
         <v>otherMarkup</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C185" t="s">
         <v>478</v>
       </c>
-      <c r="D182" t="s">
+      <c r="D185" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B183" t="str">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B186" t="str">
         <f t="shared" si="16"/>
         <v>otherDiscount</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C186" t="s">
         <v>479</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D186" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B184" t="str">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B187" t="str">
         <f t="shared" si="16"/>
         <v>otherPrice</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C187" t="s">
         <v>480</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D187" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A186" t="s">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
         <v>470</v>
       </c>
-      <c r="B186" s="6" t="str">
-        <f>C186&amp;D186&amp;E186</f>
+      <c r="B189" s="6" t="str">
+        <f>C189&amp;D189&amp;E189</f>
         <v>PizzaPicadilly.pizzaPriceList</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C189" t="s">
         <v>15</v>
       </c>
-      <c r="D186" t="s">
+      <c r="D189" t="s">
         <v>19</v>
       </c>
-      <c r="E186" t="s">
+      <c r="E189" t="s">
         <v>157</v>
       </c>
-      <c r="F186" t="s">
+      <c r="F189" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B187" t="str">
-        <f>C187</f>
-        <v>idpizzaPriceList</v>
-      </c>
-      <c r="C187" t="s">
-        <v>158</v>
-      </c>
-      <c r="D187" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B188" t="str">
-        <f t="shared" ref="B188:B194" si="17">C188</f>
-        <v>idPizzaProduct</v>
-      </c>
-      <c r="C188" t="s">
-        <v>160</v>
-      </c>
-      <c r="D188" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B189" t="str">
-        <f t="shared" si="17"/>
-        <v>pieSize</v>
-      </c>
-      <c r="C189" t="s">
-        <v>161</v>
-      </c>
-      <c r="D189" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B190" t="str">
-        <f t="shared" si="17"/>
-        <v>pizzaCode</v>
+        <f>C190</f>
+        <v>idpizzaPriceList</v>
       </c>
       <c r="C190" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D190" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B191" t="str">
-        <f t="shared" si="17"/>
-        <v>cost</v>
+        <f t="shared" ref="B191:B197" si="17">C191</f>
+        <v>idPizzaProduct</v>
       </c>
       <c r="C191" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D191" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B192" t="str">
         <f t="shared" si="17"/>
-        <v>markup</v>
+        <v>pieSize</v>
       </c>
       <c r="C192" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D192" t="s">
-        <v>118</v>
+        <v>27</v>
       </c>
     </row>
     <row r="193" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B193" t="str">
         <f t="shared" si="17"/>
-        <v>discount</v>
+        <v>pizzaCode</v>
       </c>
       <c r="C193" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D193" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
     </row>
     <row r="194" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B194" t="str">
         <f t="shared" si="17"/>
-        <v>price</v>
+        <v>cost</v>
       </c>
       <c r="C194" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D194" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="195" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B195" s="6" t="str">
-        <f>C195&amp;D195&amp;E195</f>
-        <v>PizzaPicadilly.stateSalesTax</v>
+      <c r="B195" t="str">
+        <f t="shared" si="17"/>
+        <v>markup</v>
       </c>
       <c r="C195" t="s">
-        <v>15</v>
+        <v>165</v>
       </c>
       <c r="D195" t="s">
-        <v>19</v>
-      </c>
-      <c r="E195" t="s">
-        <v>279</v>
-      </c>
-      <c r="F195" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
     </row>
     <row r="196" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B196" t="str">
-        <f>C196</f>
-        <v>idstateTax</v>
+        <f t="shared" si="17"/>
+        <v>discount</v>
       </c>
       <c r="C196" t="s">
-        <v>280</v>
+        <v>166</v>
       </c>
       <c r="D196" t="s">
-        <v>281</v>
+        <v>118</v>
       </c>
     </row>
     <row r="197" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B197" t="str">
-        <f t="shared" ref="B197:B199" si="18">C197</f>
+        <f t="shared" si="17"/>
+        <v>price</v>
+      </c>
+      <c r="C197" t="s">
+        <v>167</v>
+      </c>
+      <c r="D197" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B198" s="6" t="str">
+        <f>C198&amp;D198&amp;E198</f>
+        <v>PizzaPicadilly.stateSalesTax</v>
+      </c>
+      <c r="C198" t="s">
+        <v>15</v>
+      </c>
+      <c r="D198" t="s">
+        <v>19</v>
+      </c>
+      <c r="E198" t="s">
+        <v>279</v>
+      </c>
+      <c r="F198" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="199" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B199" t="str">
+        <f>C199</f>
+        <v>idstateTax</v>
+      </c>
+      <c r="C199" t="s">
+        <v>280</v>
+      </c>
+      <c r="D199" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="200" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B200" t="str">
+        <f t="shared" ref="B200:B202" si="18">C200</f>
         <v>stateName</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C200" t="s">
         <v>282</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D200" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="198" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B198" t="str">
+    <row r="201" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B201" t="str">
         <f t="shared" si="18"/>
         <v>stateAbbeviation</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C201" t="s">
         <v>283</v>
       </c>
-      <c r="D198" t="s">
+      <c r="D201" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="199" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B199" t="str">
+    <row r="202" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B202" t="str">
         <f t="shared" si="18"/>
         <v>taxRate</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C202" t="s">
         <v>284</v>
       </c>
-      <c r="D199" t="s">
+      <c r="D202" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="201" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B201" s="6" t="str">
-        <f>C201&amp;D201&amp;E201</f>
+    <row r="204" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B204" s="6" t="str">
+        <f>C204&amp;D204&amp;E204</f>
         <v>PizzaPicadilly.recipe_has_Ingredients</v>
       </c>
-      <c r="C201" t="s">
+      <c r="C204" t="s">
         <v>15</v>
       </c>
-      <c r="D201" t="s">
+      <c r="D204" t="s">
         <v>19</v>
       </c>
-      <c r="E201" t="s">
+      <c r="E204" t="s">
         <v>258</v>
       </c>
-      <c r="F201" t="s">
+      <c r="F204" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="202" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B202" t="str">
-        <f>C202</f>
+    <row r="205" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B205" t="str">
+        <f>C205</f>
         <v>recipe_idRecipes</v>
       </c>
-      <c r="C202" t="s">
+      <c r="C205" t="s">
         <v>237</v>
       </c>
-      <c r="D202" t="s">
+      <c r="D205" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="203" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B203" t="str">
-        <f>C203</f>
-        <v>Ingredients_idIngredients</v>
-      </c>
-      <c r="C203" t="s">
-        <v>181</v>
-      </c>
-      <c r="D203" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="205" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B205" s="6" t="str">
-        <f>C205&amp;D205&amp;E205</f>
-        <v>PizzaPicadilly.otherProductSupplier_has_otherProduct</v>
-      </c>
-      <c r="C205" t="s">
-        <v>15</v>
-      </c>
-      <c r="D205" t="s">
-        <v>19</v>
-      </c>
-      <c r="E205" t="s">
-        <v>263</v>
-      </c>
-      <c r="F205" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="206" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B206" t="str">
         <f>C206</f>
-        <v>otherProductSupplier_idSupplier</v>
+        <v>Ingredients_idIngredients</v>
       </c>
       <c r="C206" t="s">
-        <v>264</v>
+        <v>181</v>
       </c>
       <c r="D206" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B207" t="str">
-        <f t="shared" ref="B207:B209" si="19">C207</f>
+    <row r="208" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B208" s="6" t="str">
+        <f>C208&amp;D208&amp;E208</f>
+        <v>PizzaPicadilly.otherProductSupplier_has_otherProduct</v>
+      </c>
+      <c r="C208" t="s">
+        <v>15</v>
+      </c>
+      <c r="D208" t="s">
+        <v>19</v>
+      </c>
+      <c r="E208" t="s">
+        <v>263</v>
+      </c>
+      <c r="F208" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B209" t="str">
+        <f>C209</f>
+        <v>otherProductSupplier_idSupplier</v>
+      </c>
+      <c r="C209" t="s">
+        <v>264</v>
+      </c>
+      <c r="D209" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="210" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B210" t="str">
+        <f t="shared" ref="B210:B212" si="19">C210</f>
         <v>otherProduct_idotherProducts</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C210" t="s">
         <v>199</v>
       </c>
-      <c r="D207" t="s">
+      <c r="D210" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="208" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B208" t="str">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B211" t="str">
         <f t="shared" si="19"/>
         <v>otherProductSupplier_has_otherProduct_otherProductSupplier_idSupplier</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C211" t="s">
         <v>265</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D211" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="209" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B209" t="str">
+    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B212" t="str">
         <f t="shared" si="19"/>
         <v>otherProductSupplier_has_otherProduct_otherProduct_idotherProducts</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C212" t="s">
         <v>266</v>
-      </c>
-      <c r="D209" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B211" s="6" t="str">
-        <f>C211&amp;D211&amp;E211</f>
-        <v>PizzaPicadilly.productSupplier_has_Ingredients</v>
-      </c>
-      <c r="C211" t="s">
-        <v>15</v>
-      </c>
-      <c r="D211" t="s">
-        <v>19</v>
-      </c>
-      <c r="E211" t="s">
-        <v>273</v>
-      </c>
-      <c r="F211" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B212" t="str">
-        <f>C212</f>
-        <v>productSupplier_idSupplier</v>
-      </c>
-      <c r="C212" t="s">
-        <v>274</v>
       </c>
       <c r="D212" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B213" t="str">
-        <f>C213</f>
+    <row r="214" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B214" s="6" t="str">
+        <f>C214&amp;D214&amp;E214</f>
+        <v>PizzaPicadilly.productSupplier_has_Ingredients</v>
+      </c>
+      <c r="C214" t="s">
+        <v>15</v>
+      </c>
+      <c r="D214" t="s">
+        <v>19</v>
+      </c>
+      <c r="E214" t="s">
+        <v>273</v>
+      </c>
+      <c r="F214" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="215" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B215" t="str">
+        <f>C215</f>
+        <v>productSupplier_idSupplier</v>
+      </c>
+      <c r="C215" t="s">
+        <v>274</v>
+      </c>
+      <c r="D215" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="216" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B216" t="str">
+        <f>C216</f>
         <v>Ingredients_idIngredients</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C216" t="s">
         <v>181</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D216" t="s">
         <v>75</v>
       </c>
     </row>
@@ -4520,10 +4549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-    <sheetView topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="1">
+    <sheetView topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -4595,10 +4621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4640,8 +4663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
@@ -4655,10 +4677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4723,9 +4742,6 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
@@ -4781,10 +4797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -6272,8 +6285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B19"/>
     </sheetView>
   </sheetViews>
@@ -6389,10 +6401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6477,7 +6486,6 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6577,9 +6585,6 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A8"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -6697,10 +6702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE519"/>
   <sheetViews>
-    <sheetView topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="A257" sqref="A257"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12511,8 +12513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -12633,8 +12634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G6"/>
     </sheetView>
   </sheetViews>
@@ -12826,9 +12826,6 @@
   <dimension ref="A1:M78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K32" sqref="K32:K36"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -14828,10 +14825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -14865,9 +14859,6 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -15091,9 +15082,6 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -15260,12 +15248,51 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-    <sheetView topLeftCell="E1" workbookViewId="1">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:M5"/>
     </sheetView>
   </sheetViews>
@@ -15335,58 +15362,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -15395,10 +15378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-    <sheetView topLeftCell="E1" workbookViewId="1">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>

</xml_diff>